<commit_message>
quick pass through entire manuscript
see issues #21 and #25 for more.
</commit_message>
<xml_diff>
--- a/manuscript/Hypothesis table.xlsx
+++ b/manuscript/Hypothesis table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\becky\Dropbox (Smithsonian)\GitHub\Global_Productivity\manuscript\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kteixeira/Dropbox (Smithsonian)/GitHub/ForC-db/Global_Productivity/manuscript/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA59F51-765B-4EBA-8E52-170B3CF694F5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A959DF3-F0EA-7D45-ABF8-B5FF484FE241}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19040" windowHeight="14640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KAT_6_19" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="108">
   <si>
     <t>Prediction</t>
   </si>
@@ -251,9 +251,6 @@
   </si>
   <si>
     <t>4.4. Growing season length is a better predictor than MAT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.4. Allocation to carbon fluxes varies with latitude </t>
   </si>
   <si>
     <t>L+</t>
@@ -361,6 +358,18 @@
   </si>
   <si>
     <t>I-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check that references are listed in correct rowsbetween 1.1 and 1.1.alt. I think they should be switched. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2. Allocation to carbon fluxes varies with latitude </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.3 Variability with respect to latitude is similar across fluxes. </t>
+  </si>
+  <si>
+    <t>I'm still struggling with where to put this, but I think it makes sense to group it with C allocation and possibly closure of fluxes</t>
   </si>
 </sst>
 </file>
@@ -420,12 +429,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -478,7 +493,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -578,6 +593,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1026,25 +1047,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X29"/>
+  <dimension ref="A1:X30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="67" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.1796875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="34.453125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="22.1796875" style="7" customWidth="1"/>
+    <col min="1" max="1" width="3.1640625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="34.5" style="7" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" style="7" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="5" max="13" width="6.1796875" customWidth="1"/>
+    <col min="5" max="13" width="6.1640625" customWidth="1"/>
     <col min="16" max="16" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="1:24" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:24" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="17"/>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
@@ -1062,7 +1083,7 @@
       <c r="M2" s="28"/>
       <c r="N2" s="19"/>
     </row>
-    <row r="3" spans="1:24" ht="4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" ht="4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="29"/>
       <c r="B3" s="30"/>
       <c r="C3" s="30"/>
@@ -1078,7 +1099,7 @@
       <c r="M3" s="32"/>
       <c r="N3" s="31"/>
     </row>
-    <row r="4" spans="1:24" ht="63.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" ht="65" x14ac:dyDescent="0.2">
       <c r="A4" s="14"/>
       <c r="B4" s="15" t="s">
         <v>53</v>
@@ -1126,7 +1147,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>60</v>
       </c>
@@ -1138,12 +1159,12 @@
       <c r="W5" s="47"/>
       <c r="X5" s="47"/>
     </row>
-    <row r="6" spans="1:24" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:24" ht="32" x14ac:dyDescent="0.2">
       <c r="B6" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D6" s="26" t="s">
         <v>40</v>
@@ -1176,7 +1197,10 @@
         <v>40</v>
       </c>
       <c r="N6" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
+      </c>
+      <c r="P6" s="49" t="s">
+        <v>104</v>
       </c>
       <c r="S6" s="47"/>
       <c r="T6" s="47"/>
@@ -1185,13 +1209,13 @@
       <c r="W6" s="47"/>
       <c r="X6" s="47"/>
     </row>
-    <row r="7" spans="1:24" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:24" s="4" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="11"/>
       <c r="B7" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D7" s="27" t="s">
         <v>41</v>
@@ -1224,7 +1248,7 @@
         <v>41</v>
       </c>
       <c r="N7" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="S7" s="47"/>
       <c r="T7" s="47"/>
@@ -1233,13 +1257,13 @@
       <c r="W7" s="47"/>
       <c r="X7" s="47"/>
     </row>
-    <row r="8" spans="1:24" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:24" s="4" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="11"/>
       <c r="B8" s="8" t="s">
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="C8" s="39" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D8" s="26" t="s">
         <v>41</v>
@@ -1279,22 +1303,26 @@
       <c r="W8" s="47"/>
       <c r="X8" s="47"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A9" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
+    <row r="9" spans="1:24" s="4" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A9" s="11"/>
+      <c r="B9" s="48" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="39"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="27"/>
+      <c r="P9" s="4" t="s">
+        <v>107</v>
+      </c>
       <c r="S9" s="47"/>
       <c r="T9" s="47"/>
       <c r="U9" s="47"/>
@@ -1302,47 +1330,22 @@
       <c r="W9" s="47"/>
       <c r="X9" s="47"/>
     </row>
-    <row r="10" spans="1:24" s="40" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="38"/>
-      <c r="B10" s="39" t="s">
-        <v>90</v>
-      </c>
-      <c r="C10" s="39" t="s">
-        <v>89</v>
-      </c>
-      <c r="D10" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="G10" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="H10" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="I10" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="J10" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="K10" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="L10" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="M10" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="N10" s="37" t="s">
-        <v>57</v>
-      </c>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
       <c r="S10" s="47"/>
       <c r="T10" s="47"/>
       <c r="U10" s="47"/>
@@ -1350,44 +1353,45 @@
       <c r="W10" s="47"/>
       <c r="X10" s="47"/>
     </row>
-    <row r="11" spans="1:24" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B11" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="H11" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="J11" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="K11" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="L11" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="M11" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="N11" s="13" t="s">
+    <row r="11" spans="1:24" s="40" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11" s="38"/>
+      <c r="B11" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="K11" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="L11" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="M11" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="N11" s="37" t="s">
         <v>57</v>
       </c>
       <c r="S11" s="47"/>
@@ -1397,48 +1401,46 @@
       <c r="W11" s="47"/>
       <c r="X11" s="47"/>
     </row>
-    <row r="12" spans="1:24" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="41" t="s">
-        <v>103</v>
+    <row r="12" spans="1:24" ht="48" x14ac:dyDescent="0.2">
+      <c r="B12" s="7" t="s">
+        <v>77</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>40</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="G12" s="13" t="s">
         <v>40</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>104</v>
+        <v>40</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="K12" s="13" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="L12" s="13" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="M12" s="13" t="s">
         <v>40</v>
       </c>
       <c r="N12" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="O12" s="42"/>
-      <c r="P12" s="42"/>
+        <v>57</v>
+      </c>
       <c r="S12" s="47"/>
       <c r="T12" s="47"/>
       <c r="U12" s="47"/>
@@ -1446,63 +1448,74 @@
       <c r="W12" s="47"/>
       <c r="X12" s="47"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A13" s="10" t="s">
+    <row r="13" spans="1:24" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="K13" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="L13" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="M13" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="N13" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="O13" s="42"/>
+      <c r="P13" s="42"/>
+      <c r="S13" s="47"/>
+      <c r="T13" s="47"/>
+      <c r="U13" s="47"/>
+      <c r="V13" s="47"/>
+      <c r="W13" s="47"/>
+      <c r="X13" s="47"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-    </row>
-    <row r="14" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="44" t="s">
-        <v>77</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="I14" s="13" t="s">
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+    </row>
+    <row r="15" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="44" t="s">
         <v>76</v>
-      </c>
-      <c r="J14" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="K14" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="L14" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="M14" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="N14" s="13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B15" s="7" t="s">
-        <v>87</v>
       </c>
       <c r="D15" s="13" t="s">
         <v>54</v>
@@ -1520,27 +1533,27 @@
         <v>40</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="J15" s="13" t="s">
         <v>40</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L15" s="13" t="s">
         <v>40</v>
       </c>
       <c r="M15" s="13" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="N15" s="13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="29" x14ac:dyDescent="0.35">
-      <c r="B16" s="45" t="s">
-        <v>95</v>
+    <row r="16" spans="1:24" ht="48" x14ac:dyDescent="0.2">
+      <c r="B16" s="7" t="s">
+        <v>86</v>
       </c>
       <c r="D16" s="13" t="s">
         <v>54</v>
@@ -1555,272 +1568,270 @@
         <v>40</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="I16" s="13" t="s">
         <v>40</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="K16" s="13" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="L16" s="13" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="M16" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="N16" s="13"/>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A17" s="10" t="s">
+      <c r="N16" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" ht="32" x14ac:dyDescent="0.2">
+      <c r="B17" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="J17" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="K17" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="L17" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="M17" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="N17" s="13"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="N17" s="13"/>
-    </row>
-    <row r="18" spans="1:23" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="41" t="s">
+      <c r="N18" s="13"/>
+    </row>
+    <row r="19" spans="1:23" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="J19" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="K19" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="L19" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="M19" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="N19" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="P19" t="s">
+        <v>65</v>
+      </c>
+      <c r="W19" s="43"/>
+    </row>
+    <row r="20" spans="1:23" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="D18" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="H18" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="I18" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="J18" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="K18" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="L18" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="M18" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="N18" s="13" t="s">
+      <c r="D20" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="J20" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="K20" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="L20" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="M20" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="N20" s="13"/>
+    </row>
+    <row r="21" spans="1:23" ht="32" x14ac:dyDescent="0.2">
+      <c r="B21" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="J21" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="K21" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="L21" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="M21" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="N21" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="P18" t="s">
-        <v>65</v>
-      </c>
-      <c r="W18" s="43"/>
-    </row>
-    <row r="19" spans="1:23" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="41" t="s">
-        <v>97</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="H19" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="I19" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="J19" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="K19" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="L19" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="M19" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="N19" s="13"/>
-    </row>
-    <row r="20" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B20" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="H20" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="I20" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="J20" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="K20" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="L20" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="M20" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="N20" s="13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23" ht="29" x14ac:dyDescent="0.35">
-      <c r="B21" s="7" t="s">
+    </row>
+    <row r="22" spans="1:23" ht="32" x14ac:dyDescent="0.2">
+      <c r="B22" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="H21" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="I21" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="J21" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="K21" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="L21" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="M21" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="N21" s="13"/>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A22" s="10" t="s">
+      <c r="C22" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J22" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="K22" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="L22" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="M22" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="N22" s="13"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A23" s="10" t="s">
         <v>66</v>
-      </c>
-      <c r="N22" s="13"/>
-      <c r="P22" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A23" s="10"/>
-      <c r="B23" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="D23" t="s">
-        <v>69</v>
-      </c>
-      <c r="E23" t="s">
-        <v>58</v>
-      </c>
-      <c r="F23" t="s">
-        <v>58</v>
-      </c>
-      <c r="G23" t="s">
-        <v>40</v>
-      </c>
-      <c r="H23" t="s">
-        <v>58</v>
-      </c>
-      <c r="I23" t="s">
-        <v>40</v>
-      </c>
-      <c r="J23" t="s">
-        <v>58</v>
-      </c>
-      <c r="K23" t="s">
-        <v>58</v>
-      </c>
-      <c r="L23" t="s">
-        <v>58</v>
-      </c>
-      <c r="M23" t="s">
-        <v>58</v>
       </c>
       <c r="N23" s="13"/>
       <c r="P23" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
+        <v>68</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="10"/>
       <c r="B24" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>82</v>
       </c>
       <c r="D24" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="E24" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="F24" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="G24" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="H24" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="I24" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="J24" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="K24" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="L24" t="s">
         <v>58</v>
@@ -1829,118 +1840,158 @@
         <v>58</v>
       </c>
       <c r="N24" s="13"/>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="P24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="10"/>
       <c r="B25" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D25" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" t="s">
+        <v>58</v>
+      </c>
+      <c r="H25" t="s">
+        <v>40</v>
+      </c>
+      <c r="I25" t="s">
+        <v>58</v>
+      </c>
+      <c r="J25" t="s">
+        <v>40</v>
+      </c>
+      <c r="K25" t="s">
+        <v>40</v>
+      </c>
+      <c r="L25" t="s">
+        <v>58</v>
+      </c>
+      <c r="M25" t="s">
+        <v>58</v>
+      </c>
+      <c r="N25" s="13"/>
+    </row>
+    <row r="26" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="10"/>
+      <c r="B26" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" t="s">
+        <v>58</v>
+      </c>
+      <c r="F26" t="s">
+        <v>58</v>
+      </c>
+      <c r="G26" t="s">
+        <v>40</v>
+      </c>
+      <c r="H26" t="s">
+        <v>58</v>
+      </c>
+      <c r="I26" t="s">
+        <v>40</v>
+      </c>
+      <c r="J26" t="s">
+        <v>58</v>
+      </c>
+      <c r="K26" t="s">
+        <v>58</v>
+      </c>
+      <c r="L26" t="s">
+        <v>58</v>
+      </c>
+      <c r="M26" t="s">
+        <v>58</v>
+      </c>
+      <c r="N26" s="13"/>
+    </row>
+    <row r="27" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="29"/>
+      <c r="B27" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="D25" t="s">
-        <v>41</v>
-      </c>
-      <c r="E25" t="s">
-        <v>58</v>
-      </c>
-      <c r="F25" t="s">
-        <v>58</v>
-      </c>
-      <c r="G25" t="s">
-        <v>40</v>
-      </c>
-      <c r="H25" t="s">
-        <v>58</v>
-      </c>
-      <c r="I25" t="s">
-        <v>40</v>
-      </c>
-      <c r="J25" t="s">
-        <v>58</v>
-      </c>
-      <c r="K25" t="s">
-        <v>58</v>
-      </c>
-      <c r="L25" t="s">
-        <v>58</v>
-      </c>
-      <c r="M25" t="s">
-        <v>58</v>
-      </c>
-      <c r="N25" s="13"/>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A26" s="29"/>
-      <c r="B26" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="C26" s="30"/>
-      <c r="D26" s="31" t="s">
+      <c r="C27" s="30"/>
+      <c r="D27" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="E26" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="F26" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="G26" t="s">
-        <v>58</v>
-      </c>
-      <c r="H26" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="I26" t="s">
-        <v>58</v>
-      </c>
-      <c r="J26" t="s">
-        <v>58</v>
-      </c>
-      <c r="K26" s="36" t="s">
-        <v>40</v>
-      </c>
-      <c r="L26" t="s">
-        <v>58</v>
-      </c>
-      <c r="M26" t="s">
-        <v>58</v>
-      </c>
-      <c r="N26" s="46"/>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A27" s="29"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
-      <c r="K27" s="36"/>
-      <c r="L27" s="31"/>
-      <c r="M27" s="31"/>
-      <c r="N27" s="31"/>
-    </row>
-    <row r="28" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="20"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="22"/>
-      <c r="L28" s="22"/>
-      <c r="M28" s="22"/>
-      <c r="N28" s="22"/>
-    </row>
-    <row r="29" spans="1:23" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+      <c r="E27" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="G27" t="s">
+        <v>58</v>
+      </c>
+      <c r="H27" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="I27" t="s">
+        <v>58</v>
+      </c>
+      <c r="J27" t="s">
+        <v>58</v>
+      </c>
+      <c r="K27" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="L27" t="s">
+        <v>58</v>
+      </c>
+      <c r="M27" t="s">
+        <v>58</v>
+      </c>
+      <c r="N27" s="46"/>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A28" s="29"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="31"/>
+      <c r="K28" s="36"/>
+      <c r="L28" s="31"/>
+      <c r="M28" s="31"/>
+      <c r="N28" s="31"/>
+    </row>
+    <row r="29" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="20"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="22"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="22"/>
+      <c r="N29" s="22"/>
+    </row>
+    <row r="30" spans="1:23" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="S5:X12"/>
+    <mergeCell ref="S5:X13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1956,9 +2007,9 @@
       <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1967,7 +2018,7 @@
       </c>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -2000,7 +2051,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -2020,7 +2071,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -2040,7 +2091,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -2060,7 +2111,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -2080,7 +2131,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -2088,12 +2139,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -2110,22 +2161,22 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="4" t="s">
         <v>9</v>
@@ -2134,7 +2185,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="4" t="s">
         <v>10</v>
@@ -2143,7 +2194,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
         <v>11</v>
@@ -2152,12 +2203,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="4" t="s">
         <v>15</v>
@@ -2166,7 +2217,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="4" t="s">
         <v>16</v>
@@ -2175,7 +2226,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="4" t="s">
         <v>17</v>
@@ -2184,12 +2235,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="4" t="s">
         <v>18</v>
@@ -2198,7 +2249,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="4" t="s">
         <v>19</v>
@@ -2207,7 +2258,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="4" t="s">
         <v>20</v>
@@ -2216,12 +2267,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="4" t="s">
         <v>21</v>
@@ -2230,7 +2281,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="4" t="s">
         <v>22</v>
@@ -2239,7 +2290,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="4" t="s">
         <v>23</v>
@@ -2248,17 +2299,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="4" t="s">
         <v>25</v>
@@ -2267,7 +2318,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
       <c r="B34" s="4" t="s">
         <v>26</v>
@@ -2276,7 +2327,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
       <c r="B35" s="4" t="s">
         <v>27</v>
@@ -2285,7 +2336,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
       <c r="B36" s="4" t="s">
         <v>28</v>
@@ -2294,7 +2345,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
       <c r="B37" s="4" t="s">
         <v>29</v>
@@ -2303,7 +2354,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
       <c r="B38" s="4" t="s">
         <v>30</v>

</xml_diff>